<commit_message>
started fixing bugs from the big refactoring; for now it's going until the mmenu screen but it doesn't make the transition; at least it hasn't got runtime errors; next will have to also refactor ScriptMixin to simplify the logic and conform with the latest Compute() return values
</commit_message>
<xml_diff>
--- a/debug_lines.xlsx
+++ b/debug_lines.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>mvvm_core</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>script</t>
+  </si>
+  <si>
+    <t>AICI pui linia, in functie de intervalul (coloana A) unde se gaseste, in F iti apare linia unde sa te uiti in fisierul respectiv</t>
+  </si>
+  <si>
+    <t>1 am pus ca sa nu scrie INVALID la F, dar ar trebui scris nr de linii din &lt;&gt;JS script de QUX</t>
   </si>
 </sst>
 </file>
@@ -365,107 +371,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>A1+D1</f>
-        <v>758</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1101</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F7" si="0">IF(IF(E2&gt;0,E2-A2-5,0)&lt;D2,IF(E2&gt;0,E2-A2-5,0),"INVALID")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+D2</f>
+        <v>1101</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f t="shared" ref="A3:A8" si="0">A2+D2</f>
-        <v>772</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A9" si="1">A3+D3</f>
+        <v>1115</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="F4">
         <f t="shared" si="0"/>
-        <v>773</v>
-      </c>
-      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="1"/>
+        <v>1116</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="D5">
+        <v>447</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="0"/>
-        <v>1228</v>
-      </c>
-      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="1"/>
+        <v>1563</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="D6">
+        <v>783</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="0"/>
-        <v>2012</v>
-      </c>
-      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>2346</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="D6">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="D7">
+        <v>596</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="0"/>
-        <v>2598</v>
-      </c>
-      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>2942</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="D7">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>2960</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D8">
+        <v>496</v>
+      </c>
+      <c r="F8">
+        <f>IF(IF(E8&gt;0,E8-A8-5,0)&lt;D8,IF(E8&gt;0,E8-A8-5,0),"INVALID")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>3438</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="D8">
-        <v>0</v>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f>IF(IF(E9&gt;0,E9-A9-5,0)&lt;D9,IF(E9&gt;0,E9-A9-5,0),"INVALID")</f>
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed some bugs, for MVVM working on SmartBasket on to the main menu; there was an infinite loop which had to be fixed, but also implemented some QUX transition notifier and some from-js-script result handling code
</commit_message>
<xml_diff>
--- a/debug_lines.xlsx
+++ b/debug_lines.xlsx
@@ -374,7 +374,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,7 +399,7 @@
         <v>1101</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F7" si="0">IF(IF(E2&gt;0,E2-A2-5,0)&lt;D2,IF(E2&gt;0,E2-A2-5,0),"INVALID")</f>
+        <f>IF(AND(IF(E2&gt;0,E2-A2,0)&lt;D2, IF(E2&gt;0,E2-A2,0)&gt;=0),IF(E2&gt;0,E2-A2,0),"INVALID")</f>
         <v>0</v>
       </c>
     </row>
@@ -415,7 +415,7 @@
         <v>14</v>
       </c>
       <c r="F3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F3:F9" si="0">IF(AND(IF(E3&gt;0,E3-A3,0)&lt;D3, IF(E3&gt;0,E3-A3,0)&gt;=0),IF(E3&gt;0,E3-A3,0),"INVALID")</f>
         <v>0</v>
       </c>
     </row>
@@ -495,7 +495,7 @@
         <v>496</v>
       </c>
       <c r="F8">
-        <f>IF(IF(E8&gt;0,E8-A8-5,0)&lt;D8,IF(E8&gt;0,E8-A8-5,0),"INVALID")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -511,7 +511,7 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <f>IF(IF(E9&gt;0,E9-A9-5,0)&lt;D9,IF(E9&gt;0,E9-A9-5,0),"INVALID")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I9" t="s">

</xml_diff>

<commit_message>
refactorized views to be specified as meta (dictionary in views.js) and not as classes; this simplified things pretty well, so it's a sign it was a good design decision; tested some things, is seems it works; if any bug left, will be fixed on the following commits
</commit_message>
<xml_diff>
--- a/debug_lines.xlsx
+++ b/debug_lines.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -374,7 +375,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,7 +397,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1101</v>
+        <v>1247</v>
       </c>
       <c r="F2">
         <f>IF(AND(IF(E2&gt;0,E2-A2,0)&lt;D2, IF(E2&gt;0,E2-A2,0)&gt;=0),IF(E2&gt;0,E2-A2,0),"INVALID")</f>
@@ -406,7 +407,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+D2</f>
-        <v>1101</v>
+        <v>1247</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -422,7 +423,7 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A9" si="1">A3+D3</f>
-        <v>1115</v>
+        <v>1261</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -438,7 +439,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="1"/>
-        <v>1116</v>
+        <v>1262</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -454,7 +455,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="1"/>
-        <v>1563</v>
+        <v>1709</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -470,13 +471,13 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="1"/>
-        <v>2346</v>
+        <v>2492</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="D7">
-        <v>596</v>
+        <v>435</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
@@ -486,13 +487,13 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="1"/>
-        <v>2942</v>
+        <v>2927</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="D8">
-        <v>496</v>
+        <v>315</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
@@ -502,7 +503,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="1"/>
-        <v>3438</v>
+        <v>3242</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
implemented initloads mechanism for replacing REST qux components on mvvm projects and tested and fixed both initloads and external-queries module; IT WORKS very nice, now !
</commit_message>
<xml_diff>
--- a/debug_lines.xlsx
+++ b/debug_lines.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>mvvm_core</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>1 am pus ca sa nu scrie INVALID la F, dar ar trebui scris nr de linii din &lt;&gt;JS script de QUX</t>
+  </si>
+  <si>
+    <t>initloads</t>
   </si>
 </sst>
 </file>
@@ -371,16 +374,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -396,33 +400,33 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="str">
+        <v>1473</v>
+      </c>
+      <c r="F2">
         <f>IF(AND(IF(E2&gt;0,E2-A2,0)&lt;D2, IF(E2&gt;0,E2-A2,0)&gt;=0),IF(E2&gt;0,E2-A2,0),"INVALID")</f>
-        <v>INVALID</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+D2</f>
-        <v>0</v>
+        <v>1473</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F9" si="0">IF(AND(IF(E3&gt;0,E3-A3,0)&lt;D3, IF(E3&gt;0,E3-A3,0)&gt;=0),IF(E3&gt;0,E3-A3,0),"INVALID")</f>
+        <f t="shared" ref="F3:F10" si="0">IF(AND(IF(E3&gt;0,E3-A3,0)&lt;D3, IF(E3&gt;0,E3-A3,0)&gt;=0),IF(E3&gt;0,E3-A3,0),"INVALID")</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A9" si="1">A3+D3</f>
-        <v>14</v>
+        <f t="shared" ref="A4:A8" si="1">A3+D3</f>
+        <v>1474</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -438,13 +442,13 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>1475</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="D5">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -454,13 +458,13 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="1"/>
-        <v>462</v>
+        <v>1923</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="D6">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -470,7 +474,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="1"/>
-        <v>1245</v>
+        <v>2708</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -486,13 +490,13 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="1"/>
-        <v>1680</v>
+        <v>3143</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="D8">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
@@ -501,20 +505,36 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="1"/>
-        <v>1995</v>
+        <f>A8+D8</f>
+        <v>3464</v>
       </c>
       <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <f>IF(AND(IF(E10&gt;0,E10-A10,0)&lt;D10, IF(E10&gt;0,E10-A10,0)&gt;=0),IF(E10&gt;0,E10-A10,0),"INVALID")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>A9+D9</f>
+        <v>3478</v>
+      </c>
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>1</v>
       </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="F10" t="str">
+        <f>IF(AND(IF(E11&gt;0,E11-A11,0)&lt;D11, IF(E11&gt;0,E11-A11,0)&gt;=0),IF(E11&gt;0,E11-A11,0),"INVALID")</f>
+        <v>INVALID</v>
+      </c>
+      <c r="I10" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>